<commit_message>
Update to value lookups for demographics questions.
</commit_message>
<xml_diff>
--- a/assets/documents/outcome_measures_import.xlsx
+++ b/assets/documents/outcome_measures_import.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3804" windowHeight="2700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3804" windowHeight="2700" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -163,9 +163,6 @@
     <t>70-74</t>
   </si>
   <si>
-    <t>75+</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -178,9 +175,6 @@
     <t>Rocky View &amp; County Area</t>
   </si>
   <si>
-    <t>Another Province/Country</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
@@ -217,9 +211,6 @@
     <t>$200,000 +</t>
   </si>
   <si>
-    <t>I don't want to say</t>
-  </si>
-  <si>
     <t>Instructions</t>
   </si>
   <si>
@@ -263,6 +254,24 @@
   </si>
   <si>
     <t xml:space="preserve">In Tab 1, each row represents one client. For post-only surveys, always select “Post” in the first column. Enter your first client’s information using the dropdown menus. Select the cell you wish to enter data into, and you’ll see a ‘down’ arrow beside it. Click the arrow and it will give you your options. There is no dropdown for name or people in family – just type the name or value. </t>
+  </si>
+  <si>
+    <t>75 and over</t>
+  </si>
+  <si>
+    <t>No Response</t>
+  </si>
+  <si>
+    <t>Not listed</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>Prefer not to say</t>
   </si>
 </sst>
 </file>
@@ -664,7 +673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
@@ -814,15 +823,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
+            <xm:f>Data!$E$1:$E$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G1065</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
             <xm:f>Data!$D$1:$D$5</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F1165</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Data!$E$1:$E$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G1065</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -845,67 +854,67 @@
   <sheetData>
     <row r="1" spans="1:1" s="4" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -916,15 +925,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
@@ -935,19 +945,19 @@
         <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G1">
         <v>1</v>
@@ -958,53 +968,59 @@
         <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G2">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G3">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" t="s">
         <v>50</v>
       </c>
-      <c r="E4" t="s">
-        <v>54</v>
-      </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -1015,13 +1031,13 @@
         <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G5">
         <v>5</v>
@@ -1032,10 +1048,10 @@
         <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1043,26 +1059,38 @@
         <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C8" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="E9" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="E10" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
@@ -1091,7 +1119,12 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" s="2" t="s">
-        <v>45</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on value lookups for survey import.
</commit_message>
<xml_diff>
--- a/assets/documents/outcome_measures_import.xlsx
+++ b/assets/documents/outcome_measures_import.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3804" windowHeight="2700" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3804" windowHeight="2700"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -673,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H1277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,13 +784,7 @@
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Data!$F$1:$F$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H1165</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Data!$G$1:$G$5</xm:f>
@@ -805,33 +799,33 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Data!$B$1:$B$2</xm:f>
+            <xm:f>Data!$D$1:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1165</xm:sqref>
+          <xm:sqref>F2:F1165</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Data!$C$1:$C$16</xm:f>
+            <xm:f>Data!$B$1:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1165</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
-          <x14:formula1>
-            <xm:f>Data!$E$1:$E$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>G1066:G1165</xm:sqref>
+          <xm:sqref>C2:C1278</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Data!$E$1:$E$7</xm:f>
+            <xm:f>Data!$C$1:$C$17</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G1065</xm:sqref>
+          <xm:sqref>D2:D1274</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Data!$D$1:$D$5</xm:f>
+            <xm:f>Data!$E$1:$E$10</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1165</xm:sqref>
+          <xm:sqref>G2:G1274</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Data!$F$1:$F$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1277</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -927,7 +921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>